<commit_message>
Ajout de definition (anglais)
</commit_message>
<xml_diff>
--- a/knowledge/data/input/Dictionnaire.xlsx
+++ b/knowledge/data/input/Dictionnaire.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Mot</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Le dictionnaire</t>
+  </si>
+  <si>
+    <t>timonier</t>
   </si>
 </sst>
 </file>
@@ -408,11 +411,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,15 +471,15 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="str">
-        <f t="shared" ref="C3:C7" si="0">HYPERLINK("http://www.larousse.fr/encyclopedie/rechercher?q="&amp;$A3,$A3)</f>
+        <f t="shared" ref="C3:C8" si="0">HYPERLINK("http://www.larousse.fr/encyclopedie/rechercher?q="&amp;$A3,$A3)</f>
         <v>magnanime</v>
       </c>
       <c r="D3" s="1" t="str">
-        <f t="shared" ref="D3:E7" si="1">HYPERLINK("http://www.cnrtl.fr/definition/"&amp;$A3,$A3)</f>
+        <f t="shared" ref="D3:D8" si="1">HYPERLINK("http://www.cnrtl.fr/definition/"&amp;$A3,$A3)</f>
         <v>magnanime</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E7" si="2">HYPERLINK("http://www.le-dictionnaire.com/definition.php?mot="&amp;$A3,$A3)</f>
+        <f t="shared" ref="E3:E8" si="2">HYPERLINK("http://www.le-dictionnaire.com/definition.php?mot="&amp;$A3,$A3)</f>
         <v>magnanime</v>
       </c>
     </row>
@@ -552,6 +555,23 @@
       <c r="E7" s="1" t="str">
         <f t="shared" si="2"/>
         <v>fanal</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>timonier</v>
+      </c>
+      <c r="D8" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>timonier</v>
+      </c>
+      <c r="E8" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>timonier</v>
       </c>
     </row>
   </sheetData>

</xml_diff>